<commit_message>
añadir cardDetails y ajuste por cada servicio
</commit_message>
<xml_diff>
--- a/cards-test.xlsx
+++ b/cards-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Personal\Documentos personales\SCRIPT\Nuvei-Massive-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A38F28-C455-4A30-946C-53B1523606D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F4223F-490F-454C-A36A-701260148BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12373DC2-E3C6-41F0-A981-02CBE3560ADC}"/>
   </bookViews>
@@ -36,15 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>middle</t>
-  </si>
-  <si>
-    <t>last</t>
+    <t>cardNumber</t>
   </si>
 </sst>
 </file>
@@ -416,26 +410,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C1007B-24F9-43FF-9CE1-D1FD768442E8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>